<commit_message>
Update and run example downloading
</commit_message>
<xml_diff>
--- a/examples/Spreadsheet_download.xlsx
+++ b/examples/Spreadsheet_download.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Dynamical\ecodyn\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -159,6 +159,14 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -196,16 +204,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -654,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -739,9 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -769,7 +778,7 @@
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">

</xml_diff>